<commit_message>
add a Biweekly contest 90
</commit_message>
<xml_diff>
--- a/WeeklyContest/Rankings.xlsx
+++ b/WeeklyContest/Rankings.xlsx
@@ -1,25 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419EFEC3-D483-4563-9A60-AE24C1721969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-38520" yWindow="12570" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>No.</t>
   </si>
@@ -157,14 +169,70 @@
   </si>
   <si>
     <t>Higher than</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BiWC90</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2933/19748</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BiWC87</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BiWC75</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BiWC70</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BiWC69</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BiWC52</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>WC227</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2671/23589</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5214/16330</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1537/17655</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2961/15120</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2542/10364</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>724/3545</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +259,12 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -245,27 +319,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -283,7 +368,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -319,7 +404,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -388,70 +472,91 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$22</c:f>
+              <c:f>Sheet1!$A$2:$A$29</c:f>
               <c:strCache>
-                <c:ptCount val="21"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
+                  <c:v>BiWC90</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BiWC87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>BiWC75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>BiWC70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BiWC69</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>BiWC52</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>WC227</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>WC226</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="8">
                   <c:v>WC225</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
                   <c:v>WC224</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="10">
                   <c:v>WC223</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="11">
                   <c:v>WC222</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="12">
                   <c:v>WC221</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="13">
                   <c:v>WC185</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="14">
                   <c:v>WC184</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="15">
                   <c:v>WC182</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="16">
                   <c:v>WC181</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="17">
                   <c:v>WC178</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="18">
                   <c:v>WC171</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="19">
                   <c:v>WC168</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="20">
                   <c:v>WC167</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="21">
                   <c:v>WC166</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="22">
                   <c:v>WC165</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="23">
                   <c:v>WC164</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="24">
                   <c:v>WC163</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="25">
                   <c:v>WC162</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="26">
                   <c:v>WC160</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="27">
                   <c:v>WC159</c:v>
                 </c:pt>
               </c:strCache>
@@ -459,71 +564,92 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$22</c:f>
+              <c:f>Sheet1!$D$2:$D$29</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
+                  <c:v>0.85147863074741748</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88676925685700958</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.68071034905082672</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9129425092041914</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8041666666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.75472790428406022</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.795768688293371</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.76</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="8">
                   <c:v>0.65500000000000003</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
                   <c:v>0.84</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="10">
                   <c:v>0.64</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="11">
                   <c:v>0.82499999999999996</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="12">
                   <c:v>0.70500000000000007</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="13">
                   <c:v>0.80899999999999994</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="14">
                   <c:v>0.90900000000000003</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.81200000000000006</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.85799999999999998</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.82299999999999995</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.63900000000000001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.63200000000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.85699999999999998</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.73</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0.81200000000000006</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>0.85799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.82299999999999995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.63900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.63200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.85699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.81200000000000006</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>0.91300000000000003</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="24">
                   <c:v>6.4999999999999947E-2</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="25">
                   <c:v>0.71199999999999997</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="26">
                   <c:v>0.878</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="27">
                   <c:v>0.66999999999999993</c:v>
                 </c:pt>
               </c:numCache>
@@ -1327,18 +1453,24 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>61911</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>542924</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="图表 1"/>
+        <xdr:cNvPr id="2" name="图表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1618,19 +1750,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="14.75" customWidth="1"/>
+    <col min="1" max="1" width="9" style="9"/>
+    <col min="2" max="2" width="14.75" style="5" customWidth="1"/>
+    <col min="3" max="3" width="13.875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.75" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1640,322 +1775,434 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="6">
+        <f>2933/19748</f>
+        <v>0.14852136925258255</v>
+      </c>
+      <c r="D2" s="7">
+        <f t="shared" ref="D2:D8" si="0">1-C2</f>
+        <v>0.85147863074741748</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="6">
+        <f>2671/23589</f>
+        <v>0.11323074314299038</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" si="0"/>
+        <v>0.88676925685700958</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="6">
+        <f>5214/16330</f>
+        <v>0.31928965094917328</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.68071034905082672</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="6">
+        <f>1537/17655</f>
+        <v>8.7057490795808559E-2</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>0.9129425092041914</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="6">
+        <f>2961/15120</f>
+        <v>0.19583333333333333</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>0.8041666666666667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="6">
+        <f>2542/10364</f>
+        <v>0.2452720957159398</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>0.75472790428406022</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="6">
+        <f>724/3545</f>
+        <v>0.20423131170662906</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>0.795768688293371</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C9" s="6">
         <v>0.24</v>
       </c>
-      <c r="D2" s="6">
-        <f>1-C2</f>
+      <c r="D9" s="7">
+        <f>1-C9</f>
         <v>0.76</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="10" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C10" s="6">
         <v>0.34499999999999997</v>
       </c>
-      <c r="D3" s="6">
-        <f t="shared" ref="D3:D22" si="0">1-C3</f>
+      <c r="D10" s="7">
+        <f t="shared" ref="D10:D29" si="1">1-C10</f>
         <v>0.65500000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="11" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C11" s="6">
         <v>0.16</v>
       </c>
-      <c r="D4" s="6">
-        <f t="shared" si="0"/>
+      <c r="D11" s="7">
+        <f t="shared" si="1"/>
         <v>0.84</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="12" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C12" s="6">
         <v>0.36</v>
       </c>
-      <c r="D5" s="6">
-        <f t="shared" si="0"/>
+      <c r="D12" s="7">
+        <f t="shared" si="1"/>
         <v>0.64</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="13" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C13" s="6">
         <v>0.17499999999999999</v>
       </c>
-      <c r="D6" s="6">
-        <f t="shared" si="0"/>
+      <c r="D13" s="7">
+        <f t="shared" si="1"/>
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="14" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C14" s="6">
         <v>0.29499999999999998</v>
       </c>
-      <c r="D7" s="6">
-        <f t="shared" si="0"/>
+      <c r="D14" s="7">
+        <f t="shared" si="1"/>
         <v>0.70500000000000007</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="15" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C15" s="6">
         <v>0.191</v>
       </c>
-      <c r="D8" s="6">
-        <f t="shared" si="0"/>
+      <c r="D15" s="7">
+        <f t="shared" si="1"/>
         <v>0.80899999999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="16" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C16" s="6">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="D9" s="6">
-        <f t="shared" si="0"/>
+      <c r="D16" s="7">
+        <f t="shared" si="1"/>
         <v>0.90900000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C17" s="6">
         <v>0.188</v>
       </c>
-      <c r="D10" s="6">
-        <f t="shared" si="0"/>
+      <c r="D17" s="7">
+        <f t="shared" si="1"/>
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="18" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C18" s="6">
         <v>0.14199999999999999</v>
       </c>
-      <c r="D11" s="6">
-        <f t="shared" si="0"/>
+      <c r="D18" s="7">
+        <f t="shared" si="1"/>
         <v>0.85799999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="19" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C19" s="6">
         <v>0.17699999999999999</v>
       </c>
-      <c r="D12" s="6">
-        <f t="shared" si="0"/>
+      <c r="D19" s="7">
+        <f t="shared" si="1"/>
         <v>0.82299999999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="20" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C20" s="6">
         <v>0.36099999999999999</v>
       </c>
-      <c r="D13" s="6">
-        <f t="shared" si="0"/>
+      <c r="D20" s="7">
+        <f t="shared" si="1"/>
         <v>0.63900000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="21" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C21" s="6">
         <v>0.36799999999999999</v>
       </c>
-      <c r="D14" s="6">
-        <f t="shared" si="0"/>
+      <c r="D21" s="7">
+        <f t="shared" si="1"/>
         <v>0.63200000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="22" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B22" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C22" s="6">
         <v>0.14299999999999999</v>
       </c>
-      <c r="D15" s="6">
-        <f t="shared" si="0"/>
+      <c r="D22" s="7">
+        <f t="shared" si="1"/>
         <v>0.85699999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="23" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C23" s="6">
         <v>0.27</v>
       </c>
-      <c r="D16" s="6">
-        <f t="shared" si="0"/>
+      <c r="D23" s="7">
+        <f t="shared" si="1"/>
         <v>0.73</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="24" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B24" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C24" s="6">
         <v>0.188</v>
       </c>
-      <c r="D17" s="6">
-        <f t="shared" si="0"/>
+      <c r="D24" s="7">
+        <f t="shared" si="1"/>
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C25" s="8">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="D18" s="6">
-        <f t="shared" si="0"/>
+      <c r="D25" s="7">
+        <f t="shared" si="1"/>
         <v>0.91300000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="26" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B26" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C26" s="6">
         <v>0.93500000000000005</v>
       </c>
-      <c r="D19" s="6">
-        <f t="shared" si="0"/>
+      <c r="D26" s="7">
+        <f t="shared" si="1"/>
         <v>6.4999999999999947E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="27" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C27" s="6">
         <v>0.28799999999999998</v>
       </c>
-      <c r="D20" s="6">
-        <f t="shared" si="0"/>
+      <c r="D27" s="7">
+        <f t="shared" si="1"/>
         <v>0.71199999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="28" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B28" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C28" s="6">
         <v>0.122</v>
       </c>
-      <c r="D21" s="6">
-        <f t="shared" si="0"/>
+      <c r="D28" s="7">
+        <f t="shared" si="1"/>
         <v>0.878</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="29" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B29" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C29" s="6">
         <v>0.33</v>
       </c>
-      <c r="D22" s="6">
-        <f t="shared" si="0"/>
+      <c r="D29" s="7">
+        <f t="shared" si="1"/>
         <v>0.66999999999999993</v>
       </c>
     </row>

</xml_diff>